<commit_message>
search inprovements and new example template
</commit_message>
<xml_diff>
--- a/database/example.xlsx
+++ b/database/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Code\ytlinksearcher\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285B361C-4CBD-4F6A-9DEC-6083B9ACEAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D8DFCA-CAD1-4BEA-B312-1A0B59544D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87304101-A65A-449F-9943-95428A4FDD9A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Music</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Artist</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -81,14 +78,29 @@
     <t xml:space="preserve">Dynamite Beams </t>
   </si>
   <si>
-    <t>Duration</t>
+    <t>Link Rank</t>
+  </si>
+  <si>
+    <t>Duration Rank</t>
+  </si>
+  <si>
+    <t>Views Rank</t>
+  </si>
+  <si>
+    <t>Link First</t>
+  </si>
+  <si>
+    <t>Duration First</t>
+  </si>
+  <si>
+    <t>Views First</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,8 +109,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,16 +152,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,97 +477,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB58F9A9-C303-4CF2-A99C-F1D5BAC5ACBD}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="4" customWidth="1"/>
-    <col min="2" max="4" width="31.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="65.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11.140625" style="2"/>
+    <col min="1" max="1" width="9.42578125" style="3" customWidth="1"/>
+    <col min="2" max="4" width="31.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="4" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>